<commit_message>
Update all notes for today
</commit_message>
<xml_diff>
--- a/_notes/status.xlsx
+++ b/_notes/status.xlsx
@@ -194,8 +194,8 @@
   <dimension ref="A1:XFD27"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -37584,7 +37584,9 @@
       <c r="H20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="J20" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>